<commit_message>
edit menu pembelian (transaksi)
</commit_message>
<xml_diff>
--- a/POS/public/template_penjualan.xlsx
+++ b/POS/public/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00AA6ECC-9DB9-4792-B85E-6BC958F20665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71A5E1FC-C9E0-4F6D-A0A8-BF1315091AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A0B2BBA4-5050-4187-9056-DC1E6B597881}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0FCC6D7D-2CE9-431D-9D33-5C00D461B653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>user_id</t>
   </si>
@@ -36,39 +36,38 @@
     <t>pembeli</t>
   </si>
   <si>
-    <t>penjualan_tanggal</t>
-  </si>
-  <si>
-    <t>TRX0011</t>
-  </si>
-  <si>
-    <t>2025-04-12 21:09:01</t>
-  </si>
-  <si>
-    <t>TRX0012</t>
-  </si>
-  <si>
-    <t>TRX0013</t>
-  </si>
-  <si>
-    <t>Customer 21</t>
-  </si>
-  <si>
-    <t>Customer 22</t>
-  </si>
-  <si>
-    <t>Customer 23</t>
+    <t>barang_id</t>
+  </si>
+  <si>
+    <t>jumlah</t>
+  </si>
+  <si>
+    <t>Customer 16</t>
+  </si>
+  <si>
+    <t>TXR0025</t>
+  </si>
+  <si>
+    <t>TXR0024</t>
+  </si>
+  <si>
+    <t>Customer 24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,10 +95,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,75 +415,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470D786A-DDE1-4E5A-AD06-383DBD265273}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930E82D8-5B1C-4650-BB85-39697D5EBE57}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>